<commit_message>
GH ACTION Autorun Tue Jan 31 05:11:47 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles.xlsx
+++ b/Data/Revenue_ton_miles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B11CD09-42B3-4210-9EBC-B2C69B2C8F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE2B38B1-31BE-4700-9700-6E4F781C64F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-285" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -22779,11 +22779,11 @@
   <dimension ref="A1:BA54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="E77" sqref="E77"/>
+      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23191,7 +23191,7 @@
         <v>6153</v>
       </c>
       <c r="E5" s="19">
-        <v>6367</v>
+        <v>6331</v>
       </c>
       <c r="F5" s="19">
         <v>5525</v>
@@ -23352,7 +23352,7 @@
         <v>12332</v>
       </c>
       <c r="E6" s="19">
-        <v>12828</v>
+        <v>12815</v>
       </c>
       <c r="F6" s="19">
         <v>11721</v>
@@ -23513,7 +23513,7 @@
         <v>15461</v>
       </c>
       <c r="E7" s="19">
-        <v>16659</v>
+        <v>17134</v>
       </c>
       <c r="F7" s="19">
         <v>16519</v>
@@ -23674,7 +23674,7 @@
         <v>3446</v>
       </c>
       <c r="E8" s="19">
-        <v>3334</v>
+        <v>3329</v>
       </c>
       <c r="F8" s="19">
         <v>2939</v>
@@ -23835,7 +23835,7 @@
         <v>8779</v>
       </c>
       <c r="E9" s="19">
-        <v>9600</v>
+        <v>9621</v>
       </c>
       <c r="F9" s="19">
         <v>10236</v>
@@ -23996,7 +23996,7 @@
         <v>10324</v>
       </c>
       <c r="E10" s="19">
-        <v>11422</v>
+        <v>11361</v>
       </c>
       <c r="F10" s="19">
         <v>9753</v>
@@ -24157,7 +24157,7 @@
         <v>42671</v>
       </c>
       <c r="E11" s="19">
-        <v>46059</v>
+        <v>45981</v>
       </c>
       <c r="F11" s="19">
         <v>43485</v>
@@ -24318,7 +24318,7 @@
         <v>99166</v>
       </c>
       <c r="E12" s="8">
-        <v>106269</v>
+        <v>106572</v>
       </c>
       <c r="F12" s="8">
         <v>100178</v>
@@ -24539,7 +24539,7 @@
         <v>479.59773100000001</v>
       </c>
       <c r="E15" s="19">
-        <v>502.77114399999999</v>
+        <v>497.40997700000003</v>
       </c>
       <c r="F15" s="19">
         <v>395.98697499999997</v>
@@ -24700,7 +24700,7 @@
         <v>859.071507</v>
       </c>
       <c r="E16" s="19">
-        <v>949.00801200000001</v>
+        <v>948.40887599999996</v>
       </c>
       <c r="F16" s="19">
         <v>823.78218200000003</v>
@@ -24861,7 +24861,7 @@
         <v>464.79969</v>
       </c>
       <c r="E17" s="19">
-        <v>478.12067100000002</v>
+        <v>471.09817900000002</v>
       </c>
       <c r="F17" s="19">
         <v>457.06208900000001</v>
@@ -25022,7 +25022,7 @@
         <v>48.536772999999997</v>
       </c>
       <c r="E18" s="19">
-        <v>46.043171000000001</v>
+        <v>45.855141000000003</v>
       </c>
       <c r="F18" s="19">
         <v>41.413941000000001</v>
@@ -25183,7 +25183,7 @@
         <v>394.47357299999999</v>
       </c>
       <c r="E19" s="19">
-        <v>441.42868600000003</v>
+        <v>443.73432400000002</v>
       </c>
       <c r="F19" s="19">
         <v>476.21832499999999</v>
@@ -25344,7 +25344,7 @@
         <v>974.39878699999997</v>
       </c>
       <c r="E20" s="19">
-        <v>992.19971699999996</v>
+        <v>983.05326100000002</v>
       </c>
       <c r="F20" s="19">
         <v>896.68059200000005</v>
@@ -25505,7 +25505,7 @@
         <v>991.71514300000001</v>
       </c>
       <c r="E21" s="19">
-        <v>1082.535662</v>
+        <v>1080.2263829999999</v>
       </c>
       <c r="F21" s="19">
         <v>987.50854700000002</v>
@@ -25666,7 +25666,7 @@
         <v>4212.5932040000007</v>
       </c>
       <c r="E22" s="8">
-        <v>4492.1070630000004</v>
+        <v>4469.7861410000005</v>
       </c>
       <c r="F22" s="8">
         <v>4078.6526509999999</v>
@@ -25871,7 +25871,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26281,7 +26281,7 @@
         <v>6053</v>
       </c>
       <c r="E5" s="19">
-        <v>0</v>
+        <v>6561</v>
       </c>
       <c r="F5" s="19">
         <v>0</v>
@@ -26443,7 +26443,7 @@
         <v>12787</v>
       </c>
       <c r="E6" s="7">
-        <v>0</v>
+        <v>12896</v>
       </c>
       <c r="F6" s="7">
         <v>0</v>
@@ -26605,7 +26605,7 @@
         <v>19252</v>
       </c>
       <c r="E7" s="7">
-        <v>0</v>
+        <v>18286</v>
       </c>
       <c r="F7" s="7">
         <v>0</v>
@@ -26767,7 +26767,7 @@
         <v>4234</v>
       </c>
       <c r="E8" s="7">
-        <v>0</v>
+        <v>4016</v>
       </c>
       <c r="F8" s="7">
         <v>0</v>
@@ -26929,7 +26929,7 @@
         <v>9267</v>
       </c>
       <c r="E9" s="7">
-        <v>0</v>
+        <v>10090</v>
       </c>
       <c r="F9" s="7">
         <v>0</v>
@@ -27091,7 +27091,7 @@
         <v>14183</v>
       </c>
       <c r="E10" s="19">
-        <v>0</v>
+        <v>14249</v>
       </c>
       <c r="F10" s="19">
         <v>0</v>
@@ -27253,7 +27253,7 @@
         <v>37788</v>
       </c>
       <c r="E11" s="7">
-        <v>0</v>
+        <v>42082</v>
       </c>
       <c r="F11" s="7">
         <v>0</v>
@@ -27415,7 +27415,7 @@
         <v>103564</v>
       </c>
       <c r="E12" s="8">
-        <v>0</v>
+        <v>108180</v>
       </c>
       <c r="F12" s="8">
         <v>0</v>
@@ -27639,7 +27639,7 @@
         <v>461.63349899999997</v>
       </c>
       <c r="E15" s="19">
-        <v>0</v>
+        <v>475.56022100000001</v>
       </c>
       <c r="F15" s="19">
         <v>0</v>
@@ -27801,7 +27801,7 @@
         <v>898.30689199999995</v>
       </c>
       <c r="E16" s="7">
-        <v>0</v>
+        <v>897.56</v>
       </c>
       <c r="F16" s="7">
         <v>0</v>
@@ -27963,7 +27963,7 @@
         <v>629.26032899999996</v>
       </c>
       <c r="E17" s="7">
-        <v>0</v>
+        <v>586.90578000000005</v>
       </c>
       <c r="F17" s="7">
         <v>0</v>
@@ -28125,7 +28125,7 @@
         <v>55.839255999999999</v>
       </c>
       <c r="E18" s="7">
-        <v>0</v>
+        <v>54.280965000000002</v>
       </c>
       <c r="F18" s="7">
         <v>0</v>
@@ -28287,7 +28287,7 @@
         <v>450.92334599999998</v>
       </c>
       <c r="E19" s="7">
-        <v>0</v>
+        <v>429.74664200000001</v>
       </c>
       <c r="F19" s="7">
         <v>0</v>
@@ -28449,7 +28449,7 @@
         <v>1327.6224890000001</v>
       </c>
       <c r="E20" s="19">
-        <v>0</v>
+        <v>1329.007744</v>
       </c>
       <c r="F20" s="19">
         <v>0</v>
@@ -28611,7 +28611,7 @@
         <v>902.01369799999998</v>
       </c>
       <c r="E21" s="7">
-        <v>0</v>
+        <v>1045.0231799999999</v>
       </c>
       <c r="F21" s="7">
         <v>0</v>
@@ -28773,7 +28773,7 @@
         <v>4725.5995089999997</v>
       </c>
       <c r="E22" s="8">
-        <v>0</v>
+        <v>4818.0845319999999</v>
       </c>
       <c r="F22" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
GH ACTION Autorun Tue Feb  7 05:06:32 UTC 2023
</commit_message>
<xml_diff>
--- a/Data/Revenue_ton_miles.xlsx
+++ b/Data/Revenue_ton_miles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\planning\Reports\AAR\WebSummary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE2B38B1-31BE-4700-9700-6E4F781C64F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7AE8BC1-6E2B-48AD-A2CE-CA49C93B660D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-285" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="460" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="44" r:id="rId1"/>
@@ -22783,7 +22783,7 @@
       <selection activeCell="F45" sqref="F45"/>
       <selection pane="topRight" activeCell="F45" sqref="F45"/>
       <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
-      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23194,7 +23194,7 @@
         <v>6331</v>
       </c>
       <c r="F5" s="19">
-        <v>5525</v>
+        <v>5508</v>
       </c>
       <c r="G5" s="19">
         <v>6253</v>
@@ -23355,7 +23355,7 @@
         <v>12815</v>
       </c>
       <c r="F6" s="19">
-        <v>11721</v>
+        <v>11679</v>
       </c>
       <c r="G6" s="19">
         <v>12639</v>
@@ -23516,7 +23516,7 @@
         <v>17134</v>
       </c>
       <c r="F7" s="19">
-        <v>16519</v>
+        <v>17585</v>
       </c>
       <c r="G7" s="19">
         <v>15583</v>
@@ -23677,7 +23677,7 @@
         <v>3329</v>
       </c>
       <c r="F8" s="19">
-        <v>2939</v>
+        <v>2931</v>
       </c>
       <c r="G8" s="19">
         <v>3860</v>
@@ -23838,7 +23838,7 @@
         <v>9621</v>
       </c>
       <c r="F9" s="19">
-        <v>10236</v>
+        <v>10264</v>
       </c>
       <c r="G9" s="19">
         <v>10029</v>
@@ -23999,7 +23999,7 @@
         <v>11361</v>
       </c>
       <c r="F10" s="19">
-        <v>9753</v>
+        <v>9751</v>
       </c>
       <c r="G10" s="19">
         <v>11667</v>
@@ -24160,7 +24160,7 @@
         <v>45981</v>
       </c>
       <c r="F11" s="19">
-        <v>43485</v>
+        <v>43312</v>
       </c>
       <c r="G11" s="19">
         <v>48157</v>
@@ -24321,7 +24321,7 @@
         <v>106572</v>
       </c>
       <c r="F12" s="8">
-        <v>100178</v>
+        <v>101030</v>
       </c>
       <c r="G12" s="8">
         <v>108188</v>
@@ -24542,7 +24542,7 @@
         <v>497.40997700000003</v>
       </c>
       <c r="F15" s="19">
-        <v>395.98697499999997</v>
+        <v>393.62405899999999</v>
       </c>
       <c r="G15" s="19">
         <v>450.820018</v>
@@ -24703,7 +24703,7 @@
         <v>948.40887599999996</v>
       </c>
       <c r="F16" s="19">
-        <v>823.78218200000003</v>
+        <v>829.83137099999999</v>
       </c>
       <c r="G16" s="19">
         <v>904.29075799999998</v>
@@ -24864,7 +24864,7 @@
         <v>471.09817900000002</v>
       </c>
       <c r="F17" s="19">
-        <v>457.06208900000001</v>
+        <v>454.22706899999997</v>
       </c>
       <c r="G17" s="19">
         <v>476.22017899999997</v>
@@ -25025,7 +25025,7 @@
         <v>45.855141000000003</v>
       </c>
       <c r="F18" s="19">
-        <v>41.413941000000001</v>
+        <v>41.082461000000002</v>
       </c>
       <c r="G18" s="19">
         <v>50.463282999999997</v>
@@ -25186,7 +25186,7 @@
         <v>443.73432400000002</v>
       </c>
       <c r="F19" s="19">
-        <v>476.21832499999999</v>
+        <v>478.77222599999999</v>
       </c>
       <c r="G19" s="19">
         <v>415.86830800000001</v>
@@ -25347,7 +25347,7 @@
         <v>983.05326100000002</v>
       </c>
       <c r="F20" s="19">
-        <v>896.68059200000005</v>
+        <v>901.81813699999998</v>
       </c>
       <c r="G20" s="19">
         <v>1104.7375549999999</v>
@@ -25508,7 +25508,7 @@
         <v>1080.2263829999999</v>
       </c>
       <c r="F21" s="19">
-        <v>987.50854700000002</v>
+        <v>984.305296</v>
       </c>
       <c r="G21" s="19">
         <v>1051.9346680000001</v>
@@ -25669,7 +25669,7 @@
         <v>4469.7861410000005</v>
       </c>
       <c r="F22" s="8">
-        <v>4078.6526509999999</v>
+        <v>4083.6606189999998</v>
       </c>
       <c r="G22" s="8">
         <v>4454.3347690000001</v>
@@ -25871,7 +25871,7 @@
   <dimension ref="A1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26284,7 +26284,7 @@
         <v>6561</v>
       </c>
       <c r="F5" s="19">
-        <v>0</v>
+        <v>6099</v>
       </c>
       <c r="G5" s="19">
         <v>0</v>
@@ -26446,7 +26446,7 @@
         <v>12896</v>
       </c>
       <c r="F6" s="7">
-        <v>0</v>
+        <v>12320</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -26608,7 +26608,7 @@
         <v>18286</v>
       </c>
       <c r="F7" s="7">
-        <v>0</v>
+        <v>16756</v>
       </c>
       <c r="G7" s="7">
         <v>0</v>
@@ -26770,7 +26770,7 @@
         <v>4016</v>
       </c>
       <c r="F8" s="7">
-        <v>0</v>
+        <v>4088</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -26932,7 +26932,7 @@
         <v>10090</v>
       </c>
       <c r="F9" s="7">
-        <v>0</v>
+        <v>10992</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -27094,7 +27094,7 @@
         <v>14249</v>
       </c>
       <c r="F10" s="19">
-        <v>0</v>
+        <v>13323</v>
       </c>
       <c r="G10" s="19">
         <v>0</v>
@@ -27256,7 +27256,7 @@
         <v>42082</v>
       </c>
       <c r="F11" s="7">
-        <v>0</v>
+        <v>39355</v>
       </c>
       <c r="G11" s="7">
         <v>0</v>
@@ -27418,7 +27418,7 @@
         <v>108180</v>
       </c>
       <c r="F12" s="8">
-        <v>0</v>
+        <v>102933</v>
       </c>
       <c r="G12" s="8">
         <v>0</v>
@@ -27642,7 +27642,7 @@
         <v>475.56022100000001</v>
       </c>
       <c r="F15" s="19">
-        <v>0</v>
+        <v>456.74024700000001</v>
       </c>
       <c r="G15" s="19">
         <v>0</v>
@@ -27804,7 +27804,7 @@
         <v>897.56</v>
       </c>
       <c r="F16" s="7">
-        <v>0</v>
+        <v>847.61459400000001</v>
       </c>
       <c r="G16" s="7">
         <v>0</v>
@@ -27966,7 +27966,7 @@
         <v>586.90578000000005</v>
       </c>
       <c r="F17" s="7">
-        <v>0</v>
+        <v>463.67180500000001</v>
       </c>
       <c r="G17" s="7">
         <v>0</v>
@@ -28128,7 +28128,7 @@
         <v>54.280965000000002</v>
       </c>
       <c r="F18" s="7">
-        <v>0</v>
+        <v>52.335751000000002</v>
       </c>
       <c r="G18" s="7">
         <v>0</v>
@@ -28290,7 +28290,7 @@
         <v>429.74664200000001</v>
       </c>
       <c r="F19" s="7">
-        <v>0</v>
+        <v>462.15990099999999</v>
       </c>
       <c r="G19" s="7">
         <v>0</v>
@@ -28452,7 +28452,7 @@
         <v>1329.007744</v>
       </c>
       <c r="F20" s="19">
-        <v>0</v>
+        <v>1284.4992119999999</v>
       </c>
       <c r="G20" s="19">
         <v>0</v>
@@ -28614,7 +28614,7 @@
         <v>1045.0231799999999</v>
       </c>
       <c r="F21" s="7">
-        <v>0</v>
+        <v>963.02672500000006</v>
       </c>
       <c r="G21" s="7">
         <v>0</v>
@@ -28776,7 +28776,7 @@
         <v>4818.0845319999999</v>
       </c>
       <c r="F22" s="8">
-        <v>0</v>
+        <v>4530.0482349999993</v>
       </c>
       <c r="G22" s="8">
         <v>0</v>

</xml_diff>